<commit_message>
remove weird kid ideas (pear123) and replace with numeric (idXX)
</commit_message>
<xml_diff>
--- a/data/expt_2/raw_transcripts/game28.xlsx
+++ b/data/expt_2/raw_transcripts/game28.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Now?</t>
   </si>
   <si>
-    <t xml:space="preserve">pear124</t>
+    <t xml:space="preserve">id75</t>
   </si>
   <si>
     <t xml:space="preserve"> Alright, so we're going to play a super fun matching game, but before that we have to play a bubble popping game.</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve"> Yes, so you guys are going to touch the arrow on your screen and press and touch the bubbles to make them pop.</t>
   </si>
   <si>
-    <t xml:space="preserve">apple123</t>
+    <t xml:space="preserve">id74</t>
   </si>
   <si>
     <t xml:space="preserve"> Good job, yeah, you guys know.</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Now what.</t>
   </si>
   <si>
-    <t xml:space="preserve">I'm gonna wait for [apple123] to be done.</t>
+    <t xml:space="preserve">I'm gonna wait for [id74] to be done.</t>
   </si>
   <si>
     <t xml:space="preserve"> Great job, you both did amazing.</t>
@@ -103,10 +103,10 @@
     <t xml:space="preserve"> Hi, Smurphy.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hi, [pear124].</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hi, [apple123].</t>
+    <t xml:space="preserve"> Hi, [id75].</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hi, [id74].</t>
   </si>
   <si>
     <t xml:space="preserve"> So, in the game,</t>
@@ -166,13 +166,13 @@
     <t xml:space="preserve">Not me.</t>
   </si>
   <si>
-    <t xml:space="preserve"> It's you, [apple123].</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> So you're going to be the teller and you're going to be the guesser, [pear124].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">So you can tell Smurphy and [pear124] which picture has the box around it.</t>
+    <t xml:space="preserve"> It's you, [id74].</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> So you're going to be the teller and you're going to be the guesser, [id75].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So you can tell Smurphy and [id75] which picture has the box around it.</t>
   </si>
   <si>
     <t xml:space="preserve">Can you describe to them?</t>
@@ -223,13 +223,13 @@
     <t xml:space="preserve">You guessed right.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, so now [apple123] is the guesser.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> And [pear124], you're the teller.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">So you can tell [apple123] which picture has the box around it.</t>
+    <t xml:space="preserve"> Okay, so now [id74] is the guesser.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> And [id75], you're the teller.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So you can tell [id74] which picture has the box around it.</t>
   </si>
   <si>
     <t xml:space="preserve">The dog.</t>
@@ -241,10 +241,10 @@
     <t xml:space="preserve">Yay!</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, so now you're the guesser, [pear124].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">and you're the teller [apple123].</t>
+    <t xml:space="preserve"> Okay, so now you're the guesser, [id75].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and you're the teller [id74].</t>
   </si>
   <si>
     <t xml:space="preserve">The boat has the box.</t>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">So you have to touch it.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, now you're the guesser, [apple123].</t>
+    <t xml:space="preserve"> Okay, now you're the guesser, [id74].</t>
   </si>
   <si>
     <t xml:space="preserve">What if we forget and you just push the different one?</t>
@@ -292,7 +292,7 @@
     <t xml:space="preserve">the christmas tree</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, now you're the guesser, [pear124], and you're the teller, [apple123].</t>
+    <t xml:space="preserve"> Okay, now you're the guesser, [id75], and you're the teller, [id74].</t>
   </si>
   <si>
     <t xml:space="preserve">The person.</t>
@@ -319,7 +319,7 @@
     <t xml:space="preserve"> Yay, good job!</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, now you're the guesser, [apple123], and you're the teller, [pear124].</t>
+    <t xml:space="preserve"> Okay, now you're the guesser, [id74], and you're the teller, [id75].</t>
   </si>
   <si>
     <t xml:space="preserve"> Eh, I don't know.</t>
@@ -400,7 +400,7 @@
     <t xml:space="preserve"> Yay, good job, you guys are doing so great.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, now you're gonna be the guesser, [apple123],</t>
+    <t xml:space="preserve"> Okay, now you're gonna be the guesser, [id74],</t>
   </si>
   <si>
     <t xml:space="preserve">and you'll be the teller.</t>
@@ -427,10 +427,10 @@
     <t xml:space="preserve">We'll try again.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, now you're gonna be the guester, [pear124].</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> You'll be the teller, [apple123].</t>
+    <t xml:space="preserve"> Okay, now you're gonna be the guester, [id75].</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You'll be the teller, [id74].</t>
   </si>
   <si>
     <t xml:space="preserve">Which one has the box around it?</t>
@@ -445,10 +445,10 @@
     <t xml:space="preserve"> Oh, good job!</t>
   </si>
   <si>
-    <t xml:space="preserve"> Now you're going to be the guesser, [apple123].</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> And you're the teller, [pear124].</t>
+    <t xml:space="preserve"> Now you're going to be the guesser, [id74].</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> And you're the teller, [id75].</t>
   </si>
   <si>
     <t xml:space="preserve">The... beaver.</t>
@@ -472,10 +472,10 @@
     <t xml:space="preserve">T</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, so now you're the guesser, [pear124], so you're going to guess.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> So now, [apple123], you tell him which one has the box around it.</t>
+    <t xml:space="preserve"> Okay, so now you're the guesser, [id75], so you're going to guess.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> So now, [id74], you tell him which one has the box around it.</t>
   </si>
   <si>
     <t xml:space="preserve">The beaver.</t>
@@ -502,7 +502,7 @@
     <t xml:space="preserve">the bat</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, now you're the guesser, [apple123], and you're the teller.</t>
+    <t xml:space="preserve"> Okay, now you're the guesser, [id74], and you're the teller.</t>
   </si>
   <si>
     <t xml:space="preserve">Tell them which one has the box?</t>
@@ -520,7 +520,7 @@
     <t xml:space="preserve">the people</t>
   </si>
   <si>
-    <t xml:space="preserve"> Okay, now you're the guesser and you're the teller, [pear124].</t>
+    <t xml:space="preserve"> Okay, now you're the guesser and you're the teller, [id75].</t>
   </si>
   <si>
     <t xml:space="preserve">Woo!</t>
@@ -681,12 +681,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -882,3257 +886,3257 @@
   <dimension ref="A1:H209"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G204" activeCellId="0" sqref="G204"/>
+      <selection pane="bottomLeft" activeCell="G207" activeCellId="0" sqref="G207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>9000</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>9000</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>10000</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>18000</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>18000</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>19000</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>19000</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>21000</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>21000</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>23000</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>23000</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="2" t="n">
         <v>27000</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>27000</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>30000</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>30000</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="2" t="n">
         <v>32000</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>32000</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="2" t="n">
         <v>35000</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>35000</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>39000</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>39000</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>44000</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>44000</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="2" t="n">
         <v>50000</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <v>50000</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="2" t="n">
         <v>52000</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>52000</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="2" t="n">
         <v>53000</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>53000</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="2" t="n">
         <v>54000</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>54000</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="2" t="n">
         <v>56000</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <v>56000</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="2" t="n">
         <v>56980</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <v>56980</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="2" t="n">
         <v>64120</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <v>64120</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="2" t="n">
         <v>68860</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>68860</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="2" t="n">
         <v>73600</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>73600</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="2" t="n">
         <v>78740</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>78740</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="2" t="n">
         <v>82420</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <v>82420</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="2" t="n">
         <v>86380</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <v>86380</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="2" t="n">
         <v>89280</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>89700</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="2" t="n">
         <v>91000</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="2" t="n">
         <v>91120</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="2" t="n">
         <v>95180</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <v>96200</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="2" t="n">
         <v>97200</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <v>97440</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="2" t="n">
         <v>98240</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <v>98800</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="2" t="n">
         <v>103760</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <v>104040</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="2" t="n">
         <v>104540</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>104640</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="2" t="n">
         <v>105140</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="2" t="n">
         <v>105520</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="2" t="n">
         <v>106240</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="2" t="n">
         <v>106380</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="2" t="n">
         <v>108100</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="2" t="n">
         <v>108400</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="2" t="n">
         <v>110900</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <v>110900</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="2" t="n">
         <v>116740</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>116740</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="2" t="n">
         <v>117940</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>117940</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="2" t="n">
         <v>118940</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="1" t="n">
+      <c r="D41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <v>118940</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="2" t="n">
         <v>122520</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="2" t="n">
         <v>122520</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="2" t="n">
         <v>129780</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>129780</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="2" t="n">
         <v>131020</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="2" t="n">
         <v>131020</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="2" t="n">
         <v>132520</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="2" t="n">
         <v>132520</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="2" t="n">
         <v>138160</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>138160</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="2" t="n">
         <v>139160</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="2" t="n">
         <v>139160</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="2" t="n">
         <v>140880</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="2" t="n">
         <v>140880</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="2" t="n">
         <v>143600</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="2" t="n">
         <v>143940</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="B50" s="2" t="n">
         <v>144240</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="2" t="n">
         <v>144620</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="B51" s="2" t="n">
         <v>145980</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="2" t="n">
         <v>145980</v>
       </c>
-      <c r="B52" s="1" t="n">
+      <c r="B52" s="2" t="n">
         <v>146820</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H52" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="2" t="n">
         <v>146820</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="B53" s="2" t="n">
         <v>148860</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="2" t="n">
         <v>149860</v>
       </c>
-      <c r="B54" s="1" t="n">
+      <c r="B54" s="2" t="n">
         <v>150540</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="2" t="n">
         <v>151440</v>
       </c>
-      <c r="B55" s="1" t="n">
+      <c r="B55" s="2" t="n">
         <v>152640</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="2" t="n">
         <v>152740</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="B56" s="2" t="n">
         <v>153440</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="2" t="n">
         <v>153740</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="2" t="n">
         <v>156100</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="1" t="n">
+      <c r="D57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="2" t="n">
         <v>157220</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="2" t="n">
         <v>158400</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="2" t="n">
         <v>158720</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="2" t="n">
         <v>161980</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="2" t="n">
         <v>162980</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="2" t="n">
         <v>163620</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="H60" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="2" t="n">
         <v>166620</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="2" t="n">
         <v>167740</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="2" t="n">
         <v>167740</v>
       </c>
-      <c r="B62" s="1" t="n">
+      <c r="B62" s="2" t="n">
         <v>170860</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="1" t="n">
+      <c r="D62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="2" t="n">
         <v>170860</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="2" t="n">
         <v>173200</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="2" t="n">
         <v>174160</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="B64" s="2" t="n">
         <v>177620</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="H64" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="2" t="n">
         <v>177620</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="B65" s="2" t="n">
         <v>179260</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="H65" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="2" t="n">
         <v>179260</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="B66" s="2" t="n">
         <v>182060</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="2" t="n">
         <v>183420</v>
       </c>
-      <c r="B67" s="1" t="n">
+      <c r="B67" s="2" t="n">
         <v>185100</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="2" t="n">
         <v>185240</v>
       </c>
-      <c r="B68" s="1" t="n">
+      <c r="B68" s="2" t="n">
         <v>187300</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="2" t="n">
         <v>187900</v>
       </c>
-      <c r="B69" s="1" t="n">
+      <c r="B69" s="2" t="n">
         <v>190740</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="2" t="n">
         <v>191540</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="2" t="n">
         <v>192140</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="2" t="n">
         <v>192500</v>
       </c>
-      <c r="B71" s="1" t="n">
+      <c r="B71" s="2" t="n">
         <v>195820</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="2" t="n">
         <v>195900</v>
       </c>
-      <c r="B72" s="1" t="n">
+      <c r="B72" s="2" t="n">
         <v>196780</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="2" t="n">
         <v>197320</v>
       </c>
-      <c r="B73" s="1" t="n">
+      <c r="B73" s="2" t="n">
         <v>199000</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="2" t="n">
         <v>200080</v>
       </c>
-      <c r="B74" s="1" t="n">
+      <c r="B74" s="2" t="n">
         <v>200840</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="2" t="n">
         <v>200840</v>
       </c>
-      <c r="B75" s="1" t="n">
+      <c r="B75" s="2" t="n">
         <v>202840</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="1" t="n">
+      <c r="D75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="2" t="n">
         <v>202840</v>
       </c>
-      <c r="B76" s="1" t="n">
+      <c r="B76" s="2" t="n">
         <v>204840</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F76" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="H76" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="2" t="n">
         <v>204840</v>
       </c>
-      <c r="B77" s="1" t="n">
+      <c r="B77" s="2" t="n">
         <v>207840</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="2" t="n">
         <v>207840</v>
       </c>
-      <c r="B78" s="1" t="n">
+      <c r="B78" s="2" t="n">
         <v>212840</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="2" t="n">
         <v>212840</v>
       </c>
-      <c r="B79" s="1" t="n">
+      <c r="B79" s="2" t="n">
         <v>214840</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E79" s="1" t="n">
+      <c r="E79" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F79" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H79" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="2" t="n">
         <v>214840</v>
       </c>
-      <c r="B80" s="1" t="n">
+      <c r="B80" s="2" t="n">
         <v>219840</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F80" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="2" t="n">
         <v>219840</v>
       </c>
-      <c r="B81" s="1" t="n">
+      <c r="B81" s="2" t="n">
         <v>221840</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="2" t="n">
         <v>221840</v>
       </c>
-      <c r="B82" s="1" t="n">
+      <c r="B82" s="2" t="n">
         <v>222840</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F82" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="H82" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="2" t="n">
         <v>222840</v>
       </c>
-      <c r="B83" s="1" t="n">
+      <c r="B83" s="2" t="n">
         <v>226840</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F83" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="2" t="n">
         <v>226840</v>
       </c>
-      <c r="B84" s="1" t="n">
+      <c r="B84" s="2" t="n">
         <v>228840</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="2" t="n">
         <v>228840</v>
       </c>
-      <c r="B85" s="1" t="n">
+      <c r="B85" s="2" t="n">
         <v>231840</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F85" s="1" t="s">
+      <c r="F85" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="2" t="n">
         <v>233840</v>
       </c>
-      <c r="B86" s="1" t="n">
+      <c r="B86" s="2" t="n">
         <v>235840</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="2" t="n">
         <v>235840</v>
       </c>
-      <c r="B87" s="1" t="n">
+      <c r="B87" s="2" t="n">
         <v>240840</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="1" t="n">
+      <c r="D87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="2" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="2" t="n">
         <v>240840</v>
       </c>
-      <c r="B88" s="1" t="n">
+      <c r="B88" s="2" t="n">
         <v>243840</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="F88" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="2" t="n">
         <v>244840</v>
       </c>
-      <c r="B89" s="1" t="n">
+      <c r="B89" s="2" t="n">
         <v>247840</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="2" t="n">
         <v>247840</v>
       </c>
-      <c r="B90" s="1" t="n">
+      <c r="B90" s="2" t="n">
         <v>248840</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F90" s="1" t="s">
+      <c r="F90" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="2" t="n">
         <v>248840</v>
       </c>
-      <c r="B91" s="1" t="n">
+      <c r="B91" s="2" t="n">
         <v>249840</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="2" t="n">
         <v>249840</v>
       </c>
-      <c r="B92" s="1" t="n">
+      <c r="B92" s="2" t="n">
         <v>253840</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="F92" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H92" s="1" t="s">
+      <c r="H92" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="2" t="n">
         <v>253840</v>
       </c>
-      <c r="B93" s="1" t="n">
+      <c r="B93" s="2" t="n">
         <v>256840</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="F93" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="2" t="n">
         <v>256840</v>
       </c>
-      <c r="B94" s="1" t="n">
+      <c r="B94" s="2" t="n">
         <v>258840</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="F94" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="2" t="n">
         <v>258840</v>
       </c>
-      <c r="B95" s="1" t="n">
+      <c r="B95" s="2" t="n">
         <v>260840</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="2" t="n">
         <v>264840</v>
       </c>
-      <c r="B96" s="1" t="n">
+      <c r="B96" s="2" t="n">
         <v>266840</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="2" t="n">
         <v>266840</v>
       </c>
-      <c r="B97" s="1" t="n">
+      <c r="B97" s="2" t="n">
         <v>268840</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="2" t="n">
         <v>268840</v>
       </c>
-      <c r="B98" s="1" t="n">
+      <c r="B98" s="2" t="n">
         <v>270840</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="2" t="n">
         <v>270840</v>
       </c>
-      <c r="B99" s="1" t="n">
+      <c r="B99" s="2" t="n">
         <v>272840</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="2" t="n">
         <v>272840</v>
       </c>
-      <c r="B100" s="1" t="n">
+      <c r="B100" s="2" t="n">
         <v>274840</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E100" s="1" t="n">
+      <c r="E100" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="F100" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="2" t="n">
         <v>284840</v>
       </c>
-      <c r="B101" s="1" t="n">
+      <c r="B101" s="2" t="n">
         <v>286840</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="2" t="n">
         <v>287840</v>
       </c>
-      <c r="B102" s="1" t="n">
+      <c r="B102" s="2" t="n">
         <v>289840</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F102" s="1" t="s">
+      <c r="F102" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="2" t="n">
         <v>289840</v>
       </c>
-      <c r="B103" s="1" t="n">
+      <c r="B103" s="2" t="n">
         <v>290840</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="2" t="n">
         <v>290840</v>
       </c>
-      <c r="B104" s="1" t="n">
+      <c r="B104" s="2" t="n">
         <v>291840</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F104" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="2" t="n">
         <v>291840</v>
       </c>
-      <c r="B105" s="1" t="n">
+      <c r="B105" s="2" t="n">
         <v>293840</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="2" t="n">
         <v>293840</v>
       </c>
-      <c r="B106" s="1" t="n">
+      <c r="B106" s="2" t="n">
         <v>296840</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="F106" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H106" s="1" t="s">
+      <c r="H106" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="2" t="n">
         <v>301840</v>
       </c>
-      <c r="B107" s="1" t="n">
+      <c r="B107" s="2" t="n">
         <v>307840</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="2" t="n">
         <v>307840</v>
       </c>
-      <c r="B108" s="1" t="n">
+      <c r="B108" s="2" t="n">
         <v>309840</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F108" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="2" t="n">
         <v>309840</v>
       </c>
-      <c r="B109" s="1" t="n">
+      <c r="B109" s="2" t="n">
         <v>310840</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="2" t="n">
         <v>310840</v>
       </c>
-      <c r="B110" s="1" t="n">
+      <c r="B110" s="2" t="n">
         <v>314840</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="F110" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="2" t="n">
         <v>314840</v>
       </c>
-      <c r="B111" s="1" t="n">
+      <c r="B111" s="2" t="n">
         <v>315840</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="2" t="n">
         <v>315840</v>
       </c>
-      <c r="B112" s="1" t="n">
+      <c r="B112" s="2" t="n">
         <v>320840</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="2" t="n">
         <v>320840</v>
       </c>
-      <c r="B113" s="1" t="n">
+      <c r="B113" s="2" t="n">
         <v>324840</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="2" t="n">
         <v>324840</v>
       </c>
-      <c r="B114" s="1" t="n">
+      <c r="B114" s="2" t="n">
         <v>326840</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="2" t="n">
         <v>326840</v>
       </c>
-      <c r="B115" s="1" t="n">
+      <c r="B115" s="2" t="n">
         <v>328840</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="2" t="n">
         <v>328840</v>
       </c>
-      <c r="B116" s="1" t="n">
+      <c r="B116" s="2" t="n">
         <v>329840</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E116" s="1" t="n">
+      <c r="E116" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="F116" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="2" t="n">
         <v>329840</v>
       </c>
-      <c r="B117" s="1" t="n">
+      <c r="B117" s="2" t="n">
         <v>330840</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F117" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H117" s="1" t="s">
+      <c r="H117" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="2" t="n">
         <v>334840</v>
       </c>
-      <c r="B118" s="1" t="n">
+      <c r="B118" s="2" t="n">
         <v>337840</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G118" s="1" t="s">
+      <c r="D118" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G118" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="2" t="n">
         <v>337840</v>
       </c>
-      <c r="B119" s="1" t="n">
+      <c r="B119" s="2" t="n">
         <v>339840</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="2" t="n">
         <v>339840</v>
       </c>
-      <c r="B120" s="1" t="n">
+      <c r="B120" s="2" t="n">
         <v>340840</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="2" t="n">
         <v>340840</v>
       </c>
-      <c r="B121" s="1" t="n">
+      <c r="B121" s="2" t="n">
         <v>342840</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="2" t="n">
         <v>342840</v>
       </c>
-      <c r="B122" s="1" t="n">
+      <c r="B122" s="2" t="n">
         <v>344840</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D122" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E122" s="1" t="n">
+      <c r="D122" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="2" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="2" t="n">
         <v>344840</v>
       </c>
-      <c r="B123" s="1" t="n">
+      <c r="B123" s="2" t="n">
         <v>347840</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="2" t="n">
         <v>347840</v>
       </c>
-      <c r="B124" s="1" t="n">
+      <c r="B124" s="2" t="n">
         <v>348840</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D124" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F124" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="2" t="n">
         <v>348840</v>
       </c>
-      <c r="B125" s="1" t="n">
+      <c r="B125" s="2" t="n">
         <v>350840</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F125" s="1" t="s">
+      <c r="F125" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H125" s="1" t="s">
+      <c r="H125" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="2" t="n">
         <v>350840</v>
       </c>
-      <c r="B126" s="1" t="n">
+      <c r="B126" s="2" t="n">
         <v>352840</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="2" t="n">
         <v>352840</v>
       </c>
-      <c r="B127" s="1" t="n">
+      <c r="B127" s="2" t="n">
         <v>354840</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D127" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="2" t="n">
         <v>354840</v>
       </c>
-      <c r="B128" s="1" t="n">
+      <c r="B128" s="2" t="n">
         <v>355840</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D128" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="2" t="n">
         <v>355840</v>
       </c>
-      <c r="B129" s="1" t="n">
+      <c r="B129" s="2" t="n">
         <v>358840</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D129" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="2" t="n">
         <v>358840</v>
       </c>
-      <c r="B130" s="1" t="n">
+      <c r="B130" s="2" t="n">
         <v>359840</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D130" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="2" t="n">
         <v>359840</v>
       </c>
-      <c r="B131" s="1" t="n">
+      <c r="B131" s="2" t="n">
         <v>361840</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D131" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="2" t="n">
         <v>361840</v>
       </c>
-      <c r="B132" s="1" t="n">
+      <c r="B132" s="2" t="n">
         <v>364840</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D132" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E132" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F132" s="1" t="s">
+      <c r="E132" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F132" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="2" t="n">
         <v>364840</v>
       </c>
-      <c r="B133" s="1" t="n">
+      <c r="B133" s="2" t="n">
         <v>365840</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D133" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F133" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H133" s="1" t="s">
+      <c r="H133" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="2" t="n">
         <v>365840</v>
       </c>
-      <c r="B134" s="1" t="n">
+      <c r="B134" s="2" t="n">
         <v>372840</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F134" s="1" t="s">
+      <c r="F134" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="2" t="n">
         <v>372840</v>
       </c>
-      <c r="B135" s="1" t="n">
+      <c r="B135" s="2" t="n">
         <v>373840</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="D135" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="2" t="n">
         <v>373840</v>
       </c>
-      <c r="B136" s="1" t="n">
+      <c r="B136" s="2" t="n">
         <v>374840</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C136" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="D136" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="2" t="n">
         <v>374840</v>
       </c>
-      <c r="B137" s="1" t="n">
+      <c r="B137" s="2" t="n">
         <v>376840</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D137" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="2" t="n">
         <v>376840</v>
       </c>
-      <c r="B138" s="1" t="n">
+      <c r="B138" s="2" t="n">
         <v>377840</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C138" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D138" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="2" t="n">
         <v>377840</v>
       </c>
-      <c r="B139" s="1" t="n">
+      <c r="B139" s="2" t="n">
         <v>378840</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="D139" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="2" t="n">
         <v>378840</v>
       </c>
-      <c r="B140" s="1" t="n">
+      <c r="B140" s="2" t="n">
         <v>381340</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C140" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="D140" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="2" t="n">
         <v>381340</v>
       </c>
-      <c r="B141" s="1" t="n">
+      <c r="B141" s="2" t="n">
         <v>385340</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="D141" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="2" t="n">
         <v>385340</v>
       </c>
-      <c r="B142" s="1" t="n">
+      <c r="B142" s="2" t="n">
         <v>388340</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="D142" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E142" s="1" t="n">
+      <c r="E142" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F142" s="1" t="s">
+      <c r="F142" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="2" t="n">
         <v>388340</v>
       </c>
-      <c r="B143" s="1" t="n">
+      <c r="B143" s="2" t="n">
         <v>390340</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="D143" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="2" t="n">
         <v>390340</v>
       </c>
-      <c r="B144" s="1" t="n">
+      <c r="B144" s="2" t="n">
         <v>391340</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C144" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="D144" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F144" s="1" t="s">
+      <c r="F144" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="2" t="n">
         <v>390340</v>
       </c>
-      <c r="B145" s="1" t="n">
+      <c r="B145" s="2" t="n">
         <v>391340</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D145" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="2" t="n">
         <v>391340</v>
       </c>
-      <c r="B146" s="1" t="n">
+      <c r="B146" s="2" t="n">
         <v>392340</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="D146" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="2" t="n">
         <v>392340</v>
       </c>
-      <c r="B147" s="1" t="n">
+      <c r="B147" s="2" t="n">
         <v>394340</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D147" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="2" t="n">
         <v>394340</v>
       </c>
-      <c r="B148" s="1" t="n">
+      <c r="B148" s="2" t="n">
         <v>395340</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D148" s="1" t="s">
+      <c r="D148" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F148" s="1" t="s">
+      <c r="F148" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H148" s="1" t="s">
+      <c r="H148" s="2" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="2" t="n">
         <v>395340</v>
       </c>
-      <c r="B149" s="1" t="n">
+      <c r="B149" s="2" t="n">
         <v>396340</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D149" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="2" t="n">
         <v>396340</v>
       </c>
-      <c r="B150" s="1" t="n">
+      <c r="B150" s="2" t="n">
         <v>397340</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C150" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D150" s="1" t="s">
+      <c r="D150" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="2" t="n">
         <v>397340</v>
       </c>
-      <c r="B151" s="1" t="n">
+      <c r="B151" s="2" t="n">
         <v>401520</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C151" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D151" s="1" t="s">
+      <c r="D151" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="2" t="n">
         <v>402160</v>
       </c>
-      <c r="B152" s="1" t="n">
+      <c r="B152" s="2" t="n">
         <v>403560</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D152" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E152" s="1" t="n">
+      <c r="D152" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E152" s="2" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="2" t="n">
         <v>404200</v>
       </c>
-      <c r="B153" s="1" t="n">
+      <c r="B153" s="2" t="n">
         <v>405520</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D153" s="1" t="s">
+      <c r="D153" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F153" s="1" t="s">
+      <c r="F153" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H153" s="1" t="s">
+      <c r="H153" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="n">
+      <c r="A154" s="2" t="n">
         <v>408440</v>
       </c>
-      <c r="B154" s="1" t="n">
+      <c r="B154" s="2" t="n">
         <v>409040</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="C154" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D154" s="1" t="s">
+      <c r="D154" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="n">
+      <c r="A155" s="2" t="n">
         <v>411140</v>
       </c>
-      <c r="B155" s="1" t="n">
+      <c r="B155" s="2" t="n">
         <v>411780</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C155" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D155" s="1" t="s">
+      <c r="D155" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
+      <c r="A156" s="2" t="n">
         <v>412380</v>
       </c>
-      <c r="B156" s="1" t="n">
+      <c r="B156" s="2" t="n">
         <v>416220</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C156" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D156" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="n">
+      <c r="A157" s="2" t="n">
         <v>416400</v>
       </c>
-      <c r="B157" s="1" t="n">
+      <c r="B157" s="2" t="n">
         <v>418220</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C157" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="D157" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="n">
+      <c r="A158" s="2" t="n">
         <v>419020</v>
       </c>
-      <c r="B158" s="1" t="n">
+      <c r="B158" s="2" t="n">
         <v>423540</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C158" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="D158" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E158" s="1" t="n">
+      <c r="E158" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F158" s="1" t="s">
+      <c r="F158" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H158" s="1" t="s">
+      <c r="H158" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="n">
+      <c r="A159" s="2" t="n">
         <v>423540</v>
       </c>
-      <c r="B159" s="1" t="n">
+      <c r="B159" s="2" t="n">
         <v>424540</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="D159" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
+      <c r="A160" s="2" t="n">
         <v>424540</v>
       </c>
-      <c r="B160" s="1" t="n">
+      <c r="B160" s="2" t="n">
         <v>425540</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C160" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D160" s="1" t="s">
+      <c r="D160" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
+      <c r="A161" s="2" t="n">
         <v>425540</v>
       </c>
-      <c r="B161" s="1" t="n">
+      <c r="B161" s="2" t="n">
         <v>432540</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C161" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D161" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E161" s="1" t="n">
+      <c r="D161" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E161" s="2" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="n">
+      <c r="A162" s="2" t="n">
         <v>432540</v>
       </c>
-      <c r="B162" s="1" t="n">
+      <c r="B162" s="2" t="n">
         <v>433540</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="C162" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D162" s="1" t="s">
+      <c r="D162" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="n">
+      <c r="A163" s="2" t="n">
         <v>433540</v>
       </c>
-      <c r="B163" s="1" t="n">
+      <c r="B163" s="2" t="n">
         <v>434540</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="C163" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D163" s="1" t="s">
+      <c r="D163" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F163" s="1" t="s">
+      <c r="F163" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H163" s="1" t="s">
+      <c r="H163" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="n">
+      <c r="A164" s="2" t="n">
         <v>434540</v>
       </c>
-      <c r="B164" s="1" t="n">
+      <c r="B164" s="2" t="n">
         <v>435540</v>
       </c>
-      <c r="C164" s="1" t="s">
+      <c r="C164" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D164" s="1" t="s">
+      <c r="D164" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="n">
+      <c r="A165" s="2" t="n">
         <v>435540</v>
       </c>
-      <c r="B165" s="1" t="n">
+      <c r="B165" s="2" t="n">
         <v>436540</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="C165" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D165" s="1" t="s">
+      <c r="D165" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="n">
+      <c r="A166" s="2" t="n">
         <v>436540</v>
       </c>
-      <c r="B166" s="1" t="n">
+      <c r="B166" s="2" t="n">
         <v>438540</v>
       </c>
-      <c r="C166" s="1" t="s">
+      <c r="C166" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D166" s="1" t="s">
+      <c r="D166" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F166" s="1" t="s">
+      <c r="F166" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="n">
+      <c r="A167" s="2" t="n">
         <v>438540</v>
       </c>
-      <c r="B167" s="1" t="n">
+      <c r="B167" s="2" t="n">
         <v>440540</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="C167" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D167" s="1" t="s">
+      <c r="D167" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F167" s="1" t="s">
+      <c r="F167" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="n">
+      <c r="A168" s="2" t="n">
         <v>440540</v>
       </c>
-      <c r="B168" s="1" t="n">
+      <c r="B168" s="2" t="n">
         <v>443540</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="C168" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="D168" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="n">
+      <c r="A169" s="2" t="n">
         <v>443540</v>
       </c>
-      <c r="B169" s="1" t="n">
+      <c r="B169" s="2" t="n">
         <v>445540</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="C169" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D169" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E169" s="1" t="n">
+      <c r="D169" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E169" s="2" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="n">
+      <c r="A170" s="2" t="n">
         <v>445540</v>
       </c>
-      <c r="B170" s="1" t="n">
+      <c r="B170" s="2" t="n">
         <v>447540</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="C170" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="D170" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F170" s="1" t="s">
+      <c r="F170" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="n">
+      <c r="A171" s="2" t="n">
         <v>447540</v>
       </c>
-      <c r="B171" s="1" t="n">
+      <c r="B171" s="2" t="n">
         <v>449540</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="C171" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D171" s="1" t="s">
+      <c r="D171" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F171" s="1" t="s">
+      <c r="F171" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="n">
+      <c r="A172" s="2" t="n">
         <v>449540</v>
       </c>
-      <c r="B172" s="1" t="n">
+      <c r="B172" s="2" t="n">
         <v>460460</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="C172" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D172" s="1" t="s">
+      <c r="D172" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F172" s="1" t="s">
+      <c r="F172" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="n">
+      <c r="A173" s="2" t="n">
         <v>460460</v>
       </c>
-      <c r="B173" s="1" t="n">
+      <c r="B173" s="2" t="n">
         <v>462720</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="C173" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D173" s="1" t="s">
+      <c r="D173" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="n">
+      <c r="A174" s="2" t="n">
         <v>462720</v>
       </c>
-      <c r="B174" s="1" t="n">
+      <c r="B174" s="2" t="n">
         <v>470000</v>
       </c>
-      <c r="C174" s="1" t="s">
+      <c r="C174" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D174" s="1" t="s">
+      <c r="D174" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F174" s="1" t="s">
+      <c r="F174" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="n">
+      <c r="A175" s="2" t="n">
         <v>470000</v>
       </c>
-      <c r="B175" s="1" t="n">
+      <c r="B175" s="2" t="n">
         <v>471000</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="C175" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D175" s="1" t="s">
+      <c r="D175" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F175" s="1" t="s">
+      <c r="F175" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H175" s="1" t="s">
+      <c r="H175" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="n">
+      <c r="A176" s="2" t="n">
         <v>471000</v>
       </c>
-      <c r="B176" s="1" t="n">
+      <c r="B176" s="2" t="n">
         <v>472000</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C176" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D176" s="1" t="s">
+      <c r="D176" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="n">
+      <c r="A177" s="2" t="n">
         <v>472000</v>
       </c>
-      <c r="B177" s="1" t="n">
+      <c r="B177" s="2" t="n">
         <v>473000</v>
       </c>
-      <c r="C177" s="1" t="s">
+      <c r="C177" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D177" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G177" s="1" t="s">
+      <c r="D177" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G177" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="n">
+      <c r="A178" s="2" t="n">
         <v>473000</v>
       </c>
-      <c r="B178" s="1" t="n">
+      <c r="B178" s="2" t="n">
         <v>481000</v>
       </c>
-      <c r="C178" s="1" t="s">
+      <c r="C178" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D178" s="1" t="s">
+      <c r="D178" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="n">
+      <c r="A179" s="2" t="n">
         <v>481000</v>
       </c>
-      <c r="B179" s="1" t="n">
+      <c r="B179" s="2" t="n">
         <v>486000</v>
       </c>
-      <c r="C179" s="1" t="s">
+      <c r="C179" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D179" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E179" s="1" t="n">
+      <c r="D179" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E179" s="2" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="n">
+      <c r="A180" s="2" t="n">
         <v>486000</v>
       </c>
-      <c r="B180" s="1" t="n">
+      <c r="B180" s="2" t="n">
         <v>487000</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="C180" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D180" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F180" s="1" t="s">
+      <c r="F180" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H180" s="1" t="s">
+      <c r="H180" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="n">
+      <c r="A181" s="2" t="n">
         <v>487000</v>
       </c>
-      <c r="B181" s="1" t="n">
+      <c r="B181" s="2" t="n">
         <v>492000</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C181" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D181" s="1" t="s">
+      <c r="D181" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F181" s="1" t="s">
+      <c r="F181" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H181" s="1" t="s">
+      <c r="H181" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="n">
+      <c r="A182" s="2" t="n">
         <v>492000</v>
       </c>
-      <c r="B182" s="1" t="n">
+      <c r="B182" s="2" t="n">
         <v>496000</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="C182" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="D182" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="n">
+      <c r="A183" s="2" t="n">
         <v>496000</v>
       </c>
-      <c r="B183" s="1" t="n">
+      <c r="B183" s="2" t="n">
         <v>498000</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="C183" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D183" s="1" t="s">
+      <c r="D183" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F183" s="1" t="s">
+      <c r="F183" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="n">
+      <c r="A184" s="2" t="n">
         <v>498000</v>
       </c>
-      <c r="B184" s="1" t="n">
+      <c r="B184" s="2" t="n">
         <v>501000</v>
       </c>
-      <c r="C184" s="1" t="s">
+      <c r="C184" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D184" s="1" t="s">
+      <c r="D184" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="n">
+      <c r="A185" s="2" t="n">
         <v>501000</v>
       </c>
-      <c r="B185" s="1" t="n">
+      <c r="B185" s="2" t="n">
         <v>503000</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="C185" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D185" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E185" s="1" t="n">
+      <c r="D185" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E185" s="2" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="1" t="n">
+      <c r="A186" s="2" t="n">
         <v>503000</v>
       </c>
-      <c r="B186" s="1" t="n">
+      <c r="B186" s="2" t="n">
         <v>504000</v>
       </c>
-      <c r="C186" s="1" t="s">
+      <c r="C186" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D186" s="1" t="s">
+      <c r="D186" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F186" s="1" t="s">
+      <c r="F186" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H186" s="1" t="s">
+      <c r="H186" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="n">
+      <c r="A187" s="2" t="n">
         <v>504000</v>
       </c>
-      <c r="B187" s="1" t="n">
+      <c r="B187" s="2" t="n">
         <v>505760</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="C187" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D187" s="1" t="s">
+      <c r="D187" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="n">
+      <c r="A188" s="2" t="n">
         <v>505760</v>
       </c>
-      <c r="B188" s="1" t="n">
+      <c r="B188" s="2" t="n">
         <v>507760</v>
       </c>
-      <c r="C188" s="1" t="s">
+      <c r="C188" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D188" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G188" s="1" t="s">
+      <c r="D188" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G188" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="1" t="n">
+      <c r="A189" s="2" t="n">
         <v>505760</v>
       </c>
-      <c r="B189" s="1" t="n">
+      <c r="B189" s="2" t="n">
         <v>507760</v>
       </c>
-      <c r="C189" s="1" t="s">
+      <c r="C189" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D189" s="1" t="s">
+      <c r="D189" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F189" s="1" t="s">
+      <c r="F189" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H189" s="1" t="s">
+      <c r="H189" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="n">
+      <c r="A190" s="2" t="n">
         <v>507760</v>
       </c>
-      <c r="B190" s="1" t="n">
+      <c r="B190" s="2" t="n">
         <v>512760</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="C190" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D190" s="1" t="s">
+      <c r="D190" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="1" t="n">
+      <c r="A191" s="2" t="n">
         <v>512760</v>
       </c>
-      <c r="B191" s="1" t="n">
+      <c r="B191" s="2" t="n">
         <v>515760</v>
       </c>
-      <c r="C191" s="1" t="s">
+      <c r="C191" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D191" s="1" t="s">
+      <c r="D191" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="1" t="n">
+      <c r="A192" s="2" t="n">
         <v>515760</v>
       </c>
-      <c r="B192" s="1" t="n">
+      <c r="B192" s="2" t="n">
         <v>516760</v>
       </c>
-      <c r="C192" s="1" t="s">
+      <c r="C192" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D192" s="1" t="s">
+      <c r="D192" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="1" t="n">
+      <c r="A193" s="2" t="n">
         <v>516760</v>
       </c>
-      <c r="B193" s="1" t="n">
+      <c r="B193" s="2" t="n">
         <v>521760</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="C193" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D193" s="1" t="s">
+      <c r="D193" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="1" t="n">
+      <c r="A194" s="2" t="n">
         <v>521760</v>
       </c>
-      <c r="B194" s="1" t="n">
+      <c r="B194" s="2" t="n">
         <v>522760</v>
       </c>
-      <c r="C194" s="1" t="s">
+      <c r="C194" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D194" s="1" t="s">
+      <c r="D194" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E194" s="1" t="n">
+      <c r="E194" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="F194" s="1" t="s">
+      <c r="F194" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="1" t="n">
+      <c r="A195" s="2" t="n">
         <v>522760</v>
       </c>
-      <c r="B195" s="1" t="n">
+      <c r="B195" s="2" t="n">
         <v>524760</v>
       </c>
-      <c r="C195" s="1" t="s">
+      <c r="C195" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D195" s="1" t="s">
+      <c r="D195" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F195" s="1" t="s">
+      <c r="F195" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H195" s="1" t="s">
+      <c r="H195" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="1" t="n">
+      <c r="A196" s="2" t="n">
         <v>525760</v>
       </c>
-      <c r="B196" s="1" t="n">
+      <c r="B196" s="2" t="n">
         <v>526760</v>
       </c>
-      <c r="C196" s="1" t="s">
+      <c r="C196" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D196" s="1" t="s">
+      <c r="D196" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="1" t="n">
+      <c r="A197" s="2" t="n">
         <v>526760</v>
       </c>
-      <c r="B197" s="1" t="n">
+      <c r="B197" s="2" t="n">
         <v>527760</v>
       </c>
-      <c r="C197" s="1" t="s">
+      <c r="C197" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D197" s="1" t="s">
+      <c r="D197" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="n">
+      <c r="A198" s="2" t="n">
         <v>527760</v>
       </c>
-      <c r="B198" s="1" t="n">
+      <c r="B198" s="2" t="n">
         <v>532760</v>
       </c>
-      <c r="C198" s="1" t="s">
+      <c r="C198" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D198" s="1" t="s">
+      <c r="D198" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="1" t="n">
+      <c r="A199" s="2" t="n">
         <v>532760</v>
       </c>
-      <c r="B199" s="1" t="n">
+      <c r="B199" s="2" t="n">
         <v>539760</v>
       </c>
-      <c r="C199" s="1" t="s">
+      <c r="C199" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D199" s="1" t="s">
+      <c r="D199" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E199" s="1" t="n">
+      <c r="E199" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="F199" s="1" t="s">
+      <c r="F199" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H199" s="1" t="s">
+      <c r="H199" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="n">
+      <c r="A200" s="2" t="n">
         <v>539760</v>
       </c>
-      <c r="B200" s="1" t="n">
+      <c r="B200" s="2" t="n">
         <v>541760</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="C200" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D200" s="1" t="s">
+      <c r="D200" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="1" t="n">
+      <c r="A201" s="2" t="n">
         <v>541760</v>
       </c>
-      <c r="B201" s="1" t="n">
+      <c r="B201" s="2" t="n">
         <v>543760</v>
       </c>
-      <c r="C201" s="1" t="s">
+      <c r="C201" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D201" s="1" t="s">
+      <c r="D201" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="n">
+      <c r="A202" s="2" t="n">
         <v>543760</v>
       </c>
-      <c r="B202" s="1" t="n">
+      <c r="B202" s="2" t="n">
         <v>545760</v>
       </c>
-      <c r="C202" s="1" t="s">
+      <c r="C202" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D202" s="1" t="s">
+      <c r="D202" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="n">
+      <c r="A203" s="2" t="n">
         <v>545760</v>
       </c>
-      <c r="B203" s="1" t="n">
+      <c r="B203" s="2" t="n">
         <v>547760</v>
       </c>
-      <c r="C203" s="1" t="s">
+      <c r="C203" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D203" s="1" t="s">
+      <c r="D203" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="1" t="n">
+      <c r="A204" s="2" t="n">
         <v>547760</v>
       </c>
-      <c r="B204" s="1" t="n">
+      <c r="B204" s="2" t="n">
         <v>549760</v>
       </c>
-      <c r="C204" s="1" t="s">
+      <c r="C204" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D204" s="1" t="s">
+      <c r="D204" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E204" s="1" t="n">
+      <c r="E204" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="F204" s="1" t="s">
+      <c r="F204" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H204" s="1" t="s">
+      <c r="H204" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="1" t="n">
+      <c r="A205" s="2" t="n">
         <v>549760</v>
       </c>
-      <c r="B205" s="1" t="n">
+      <c r="B205" s="2" t="n">
         <v>553760</v>
       </c>
-      <c r="C205" s="1" t="s">
+      <c r="C205" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D205" s="1" t="s">
+      <c r="D205" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="1" t="n">
+      <c r="A206" s="2" t="n">
         <v>553760</v>
       </c>
-      <c r="B206" s="1" t="n">
+      <c r="B206" s="2" t="n">
         <v>554760</v>
       </c>
-      <c r="C206" s="1" t="s">
+      <c r="C206" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D206" s="1" t="s">
+      <c r="D206" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1" t="n">
+      <c r="A207" s="2" t="n">
         <v>554760</v>
       </c>
-      <c r="B207" s="1" t="n">
+      <c r="B207" s="2" t="n">
         <v>555760</v>
       </c>
-      <c r="C207" s="1" t="s">
+      <c r="C207" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D207" s="1" t="s">
+      <c r="D207" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1" t="n">
+      <c r="A208" s="2" t="n">
         <v>555760</v>
       </c>
-      <c r="B208" s="1" t="n">
+      <c r="B208" s="2" t="n">
         <v>557760</v>
       </c>
-      <c r="C208" s="1" t="s">
+      <c r="C208" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D208" s="1" t="s">
+      <c r="D208" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="1" t="n">
+      <c r="A209" s="2" t="n">
         <v>557760</v>
       </c>
-      <c r="B209" s="1" t="n">
+      <c r="B209" s="2" t="n">
         <v>559760</v>
       </c>
-      <c r="C209" s="1" t="s">
+      <c r="C209" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D209" s="1" t="s">
+      <c r="D209" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>